<commit_message>
begin on kriging code
</commit_message>
<xml_diff>
--- a/childhood_obesity_2016_2017.xlsx
+++ b/childhood_obesity_2016_2017.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t xml:space="preserve">State </t>
   </si>
@@ -103,34 +103,28 @@
     <t>Montana</t>
   </si>
   <si>
-    <t>North</t>
-  </si>
-  <si>
-    <t>Carolina</t>
-  </si>
-  <si>
-    <t>Dakota</t>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>North Dakota</t>
   </si>
   <si>
     <t>Nebraska</t>
   </si>
   <si>
-    <t>New</t>
-  </si>
-  <si>
-    <t>Hampshire</t>
-  </si>
-  <si>
-    <t>Jersey</t>
-  </si>
-  <si>
-    <t>Mexico</t>
+    <t>New Hampshire</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
   </si>
   <si>
     <t>Nevada</t>
   </si>
   <si>
-    <t>York</t>
+    <t>New York</t>
   </si>
   <si>
     <t>Ohio</t>
@@ -145,13 +139,13 @@
     <t>Pennsylvania</t>
   </si>
   <si>
-    <t>Rhode</t>
-  </si>
-  <si>
-    <t>Island</t>
-  </si>
-  <si>
-    <t>South</t>
+    <t>Rhode Island</t>
+  </si>
+  <si>
+    <t>South Carolina</t>
+  </si>
+  <si>
+    <t>South Dakota</t>
   </si>
   <si>
     <t>Tennessee</t>
@@ -175,7 +169,7 @@
     <t>Wisconsin</t>
   </si>
   <si>
-    <t>West</t>
+    <t>West Virginia</t>
   </si>
   <si>
     <t>Wyoming</t>
@@ -185,7 +179,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -196,8 +190,12 @@
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,6 +206,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB0B3B2"/>
         <bgColor rgb="FFB0B3B2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -231,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -241,8 +245,11 @@
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="top"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -284,11 +291,11 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3">
-        <v>0.154</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.126</v>
+      <c r="B2" s="2">
+        <v>15.4</v>
+      </c>
+      <c r="C2" s="2">
+        <v>12.6</v>
       </c>
     </row>
     <row r="3">
@@ -559,11 +566,11 @@
       <c r="A27" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="3">
-        <v>0.262</v>
-      </c>
-      <c r="C27" s="3">
-        <v>0.261</v>
+      <c r="B27" s="2">
+        <v>26.2</v>
+      </c>
+      <c r="C27" s="2">
+        <v>26.1</v>
       </c>
     </row>
     <row r="28">
@@ -581,27 +588,27 @@
       <c r="A29" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="2">
+      <c r="B29" s="2">
         <v>12.6</v>
+      </c>
+      <c r="C29" s="3">
+        <v>13.1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="2">
+        <v>31</v>
+      </c>
+      <c r="B30" s="2">
         <v>15.8</v>
+      </c>
+      <c r="C30" s="3">
+        <v>12.5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" s="2">
         <v>16.7</v>
@@ -612,40 +619,40 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" s="2">
+        <v>33</v>
+      </c>
+      <c r="B32" s="2">
         <v>8.5</v>
+      </c>
+      <c r="C32" s="3">
+        <v>9.8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="2">
+      <c r="B33" s="2">
+        <v>14.8</v>
+      </c>
+      <c r="C33" s="3">
         <v>14.8</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C34" s="2">
+        <v>35</v>
+      </c>
+      <c r="B34" s="2">
         <v>13.1</v>
+      </c>
+      <c r="C34" s="3">
+        <v>15.1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B35" s="2">
         <v>14.5</v>
@@ -656,18 +663,18 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="2">
+        <v>37</v>
+      </c>
+      <c r="B36" s="2">
         <v>14.8</v>
+      </c>
+      <c r="C36" s="3">
+        <v>15.3</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B37" s="2">
         <v>18.6</v>
@@ -678,7 +685,7 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B38" s="2">
         <v>18.1</v>
@@ -689,7 +696,7 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B39" s="2">
         <v>10.2</v>
@@ -700,7 +707,7 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B40" s="2">
         <v>14.2</v>
@@ -711,40 +718,40 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C41" s="2">
+        <v>42</v>
+      </c>
+      <c r="B41" s="2">
         <v>19.2</v>
+      </c>
+      <c r="C41" s="3">
+        <v>16.8</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C42" s="2">
+        <v>43</v>
+      </c>
+      <c r="B42" s="2">
         <v>18.2</v>
+      </c>
+      <c r="C42" s="3">
+        <v>15.4</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C43" s="2">
+        <v>44</v>
+      </c>
+      <c r="B43" s="2">
         <v>13.0</v>
+      </c>
+      <c r="C43" s="3">
+        <v>13.6</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B44" s="2">
         <v>19.2</v>
@@ -755,7 +762,7 @@
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B45" s="2">
         <v>21.3</v>
@@ -766,7 +773,7 @@
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B46" s="2">
         <v>9.5</v>
@@ -777,7 +784,7 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B47" s="2">
         <v>14.1</v>
@@ -788,7 +795,7 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B48" s="2">
         <v>11.8</v>
@@ -799,7 +806,7 @@
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B49" s="2">
         <v>8.7</v>
@@ -810,7 +817,7 @@
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B50" s="2">
         <v>14.6</v>
@@ -821,18 +828,18 @@
     </row>
     <row r="51">
       <c r="A51" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C51" s="2">
+        <v>52</v>
+      </c>
+      <c r="B51" s="3">
         <v>19.9</v>
+      </c>
+      <c r="C51" s="4">
+        <v>20.3</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B52" s="2">
         <v>12.9</v>

</xml_diff>